<commit_message>
Wheel colors based on header color in spreadsheet.
</commit_message>
<xml_diff>
--- a/spread.xlsx
+++ b/spread.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riraa\OneDrive\Pulpit\noce\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programowanie\Fun\movie-nights-picker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B07D9AF3-2343-423A-BBDC-5A59AC8CF5B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902260A5-6DB6-4862-955A-E29E097983C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="7980" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheetgo_losowanie" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
   <si>
     <t>xero</t>
   </si>
@@ -44,9 +44,6 @@
   </si>
   <si>
     <t>p*lskie</t>
-  </si>
-  <si>
-    <t>p. vega</t>
   </si>
   <si>
     <t>koreanskie dramy</t>
@@ -197,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -213,13 +210,17 @@
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,6 +230,78 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9933FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC00FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3399"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00FFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF3333FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -265,7 +338,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -282,9 +355,46 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -355,6 +465,18 @@
       <rgbColor rgb="00333399"/>
       <rgbColor rgb="00333333"/>
     </indexedColors>
+    <mruColors>
+      <color rgb="FFFF66FF"/>
+      <color rgb="FFCC00FF"/>
+      <color rgb="FF9933FF"/>
+      <color rgb="FFCC66FF"/>
+      <color rgb="FFFF00FF"/>
+      <color rgb="FF3333FF"/>
+      <color rgb="FF0099FF"/>
+      <color rgb="FF00FFFF"/>
+      <color rgb="FFFF3399"/>
+      <color rgb="FF3333CC"/>
+    </mruColors>
   </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -548,84 +670,84 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.81640625" customWidth="1"/>
     <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="15" max="15" width="15.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>40</v>
+      <c r="H1" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="L1" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" s="15" t="s">
+        <v>39</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -636,19 +758,19 @@
       <c r="N2" s="2"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -659,57 +781,57 @@
       <c r="N3" s="2"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="2"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -717,52 +839,52 @@
       <c r="N5" s="2"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K6" s="1"/>
       <c r="L6" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
@@ -771,24 +893,24 @@
       <c r="N7" s="2"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -796,28 +918,28 @@
       <c r="N8" s="2"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>50</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -825,30 +947,30 @@
       <c r="N9" s="2"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -856,7 +978,7 @@
       <c r="N10" s="2"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -873,7 +995,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -890,7 +1012,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -907,7 +1029,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -924,7 +1046,7 @@
       <c r="N14" s="2"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -940,7 +1062,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -955,11 +1077,11 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
       <c r="N16" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -977,10 +1099,10 @@
         <v>4</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -998,10 +1120,10 @@
         <v>2</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1016,13 +1138,13 @@
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
       <c r="N19" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1040,10 +1162,10 @@
         <v>4</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1061,10 +1183,10 @@
         <v>3</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1079,13 +1201,13 @@
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1103,53 +1225,53 @@
         <v>2</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="N24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" ht="14" x14ac:dyDescent="0.3">
       <c r="N25" s="2" t="s">
         <v>2</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N26" s="3"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N27" s="3"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N28" s="3"/>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
       <c r="N35" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update colors to not cause stupid crashes
</commit_message>
<xml_diff>
--- a/spread.xlsx
+++ b/spread.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programowanie\Fun\movie-nights-picker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riraa\OneDrive\Pulpit\noce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{902260A5-6DB6-4862-955A-E29E097983C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB50338-CC91-43A7-B563-2A8178A7A830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7980" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="7125" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheetgo_losowanie" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
   <si>
     <t>xero</t>
   </si>
@@ -187,14 +187,44 @@
     <t>tiktok filmy</t>
   </si>
   <si>
-    <t>bojownicy</t>
+    <t>kamera na środku</t>
+  </si>
+  <si>
+    <t>kot w butach</t>
+  </si>
+  <si>
+    <t>aktorskie księżniczki disneya</t>
+  </si>
+  <si>
+    <t>bojownicy (buntownicy)</t>
+  </si>
+  <si>
+    <t>madds mikkellsenn</t>
+  </si>
+  <si>
+    <t>kryminalne</t>
+  </si>
+  <si>
+    <t>horrory2024</t>
+  </si>
+  <si>
+    <t>niezombie</t>
+  </si>
+  <si>
+    <t>alien</t>
+  </si>
+  <si>
+    <t>basketball</t>
+  </si>
+  <si>
+    <t>wrestling</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -219,6 +249,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="238"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -235,12 +279,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -295,13 +333,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF3333FF"/>
+        <fgColor rgb="FFFF66FF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF66FF"/>
+        <fgColor rgb="FFB09210"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDD8989"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -338,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -385,16 +429,18 @@
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -466,16 +512,16 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFDD8989"/>
+      <color rgb="FFB09210"/>
+      <color rgb="FFFEFDFE"/>
+      <color rgb="FF000000"/>
+      <color rgb="FF5C0000"/>
       <color rgb="FFFF66FF"/>
       <color rgb="FFCC00FF"/>
       <color rgb="FF9933FF"/>
       <color rgb="FFCC66FF"/>
       <color rgb="FFFF00FF"/>
-      <color rgb="FF3333FF"/>
-      <color rgb="FF0099FF"/>
-      <color rgb="FF00FFFF"/>
-      <color rgb="FFFF3399"/>
-      <color rgb="FF3333CC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -670,72 +716,71 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="I9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" customWidth="1"/>
     <col min="2" max="2" width="18" customWidth="1"/>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="19" customWidth="1"/>
-    <col min="6" max="6" width="17.81640625" customWidth="1"/>
-    <col min="8" max="8" width="11.26953125" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" customWidth="1"/>
-    <col min="12" max="12" width="13.54296875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" customWidth="1"/>
+    <col min="5" max="5" width="27.140625" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" customWidth="1"/>
+    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="19.140625" customWidth="1"/>
+    <col min="12" max="12" width="13.5703125" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="15" max="15" width="15.81640625" customWidth="1"/>
+    <col min="15" max="15" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="12" t="s">
+      <c r="F1" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="J1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="14" t="s">
+      <c r="K1" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="L1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="M1" s="14" t="s">
         <v>39</v>
       </c>
       <c r="N1" s="4"/>
       <c r="O1" s="5"/>
     </row>
-    <row r="2" spans="1:15" ht="14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="20" t="s">
+    <row r="2" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A2" s="1"/>
+      <c r="B2" s="18" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -758,10 +803,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>7</v>
-      </c>
+    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
@@ -781,7 +823,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -812,7 +854,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -839,7 +881,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -870,7 +912,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="1"/>
     </row>
-    <row r="7" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -893,7 +935,7 @@
       <c r="N7" s="2"/>
       <c r="O7" s="1"/>
     </row>
-    <row r="8" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -918,7 +960,7 @@
       <c r="N8" s="2"/>
       <c r="O8" s="1"/>
     </row>
-    <row r="9" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>47</v>
       </c>
@@ -926,9 +968,6 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>49</v>
@@ -947,7 +986,7 @@
       <c r="N9" s="2"/>
       <c r="O9" s="1"/>
     </row>
-    <row r="10" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -956,15 +995,13 @@
       <c r="D10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>52</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
         <v>49</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>53</v>
@@ -978,33 +1015,57 @@
       <c r="N10" s="2"/>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" ht="14" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>57</v>
+      </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
       <c r="N11" s="2"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="14" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
+    <row r="12" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A12" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="E12" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -1012,24 +1073,36 @@
       <c r="N12" s="2"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" ht="14" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
+    <row r="13" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A13" s="19" t="s">
+        <v>61</v>
+      </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="N13" s="2"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1046,7 +1119,7 @@
       <c r="N14" s="2"/>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1062,7 +1135,7 @@
       <c r="M15" s="1"/>
       <c r="N15" s="3"/>
     </row>
-    <row r="16" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1081,7 +1154,7 @@
       </c>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1102,7 +1175,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1123,7 +1196,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1144,7 +1217,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1165,7 +1238,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1186,7 +1259,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1207,7 +1280,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1228,7 +1301,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="N24" s="2" t="s">
         <v>20</v>
       </c>
@@ -1236,7 +1309,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="14" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
       <c r="N25" s="2" t="s">
         <v>2</v>
       </c>
@@ -1244,34 +1317,49 @@
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N27" s="3"/>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N28" s="3"/>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N27" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="O27" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N28" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
       <c r="N29" s="3"/>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
       <c r="N30" s="3"/>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="N31" s="3"/>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="N32" s="3"/>
     </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N33" s="3"/>
     </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N34" s="3"/>
     </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="14:14" x14ac:dyDescent="0.2">
       <c r="N35" s="3"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changes in color; updated data
</commit_message>
<xml_diff>
--- a/spread.xlsx
+++ b/spread.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riraa\OneDrive\Pulpit\noce\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB50338-CC91-43A7-B563-2A8178A7A830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8D2777F-2337-49B1-B6A6-425802FF2C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="7125" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="31920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheetgo_losowanie" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" iterateDelta="1E-4"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="81">
   <si>
     <t>xero</t>
   </si>
@@ -184,9 +185,6 @@
     <t>1 pokój</t>
   </si>
   <si>
-    <t>tiktok filmy</t>
-  </si>
-  <si>
     <t>kamera na środku</t>
   </si>
   <si>
@@ -218,6 +216,54 @@
   </si>
   <si>
     <t>wrestling</t>
+  </si>
+  <si>
+    <t>pętla czasowa</t>
+  </si>
+  <si>
+    <t>francuskie</t>
+  </si>
+  <si>
+    <t>baseball</t>
+  </si>
+  <si>
+    <t>gwiezdne</t>
+  </si>
+  <si>
+    <t>vincent gallo kino</t>
+  </si>
+  <si>
+    <t>dziwni nauczyciele</t>
+  </si>
+  <si>
+    <t>julia</t>
+  </si>
+  <si>
+    <t>cringe disney</t>
+  </si>
+  <si>
+    <t>Wiktoria</t>
+  </si>
+  <si>
+    <t>Real psycho</t>
+  </si>
+  <si>
+    <t>Twój stary na rybach</t>
+  </si>
+  <si>
+    <t>Sądowe</t>
+  </si>
+  <si>
+    <t>Samochodowy</t>
+  </si>
+  <si>
+    <t>syn z przyszłości</t>
+  </si>
+  <si>
+    <t>Cheetos</t>
+  </si>
+  <si>
+    <t>Filmy tiktok</t>
   </si>
 </sst>
 </file>
@@ -264,7 +310,7 @@
       <charset val="238"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -349,6 +395,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -382,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -436,6 +488,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -512,6 +567,7 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
     <mruColors>
+      <color rgb="FFFF6699"/>
       <color rgb="FFDD8989"/>
       <color rgb="FFB09210"/>
       <color rgb="FFFEFDFE"/>
@@ -521,7 +577,6 @@
       <color rgb="FFCC00FF"/>
       <color rgb="FF9933FF"/>
       <color rgb="FFCC66FF"/>
-      <color rgb="FFFF00FF"/>
     </mruColors>
   </colors>
   <extLst>
@@ -714,10 +769,10 @@
   <sheetPr>
     <tabColor rgb="FF00CC3E"/>
   </sheetPr>
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I9" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="240" zoomScaleNormal="240" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -730,12 +785,12 @@
     <col min="6" max="6" width="17.85546875" customWidth="1"/>
     <col min="8" max="8" width="22.140625" customWidth="1"/>
     <col min="10" max="10" width="19.140625" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" customWidth="1"/>
-    <col min="13" max="13" width="10" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" customWidth="1"/>
+    <col min="12" max="14" width="13.5703125" customWidth="1"/>
+    <col min="15" max="15" width="10" customWidth="1"/>
+    <col min="17" max="17" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="6" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="6" customFormat="1" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
@@ -772,13 +827,19 @@
       <c r="L1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="N1" s="23" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="N1" s="4"/>
-      <c r="O1" s="5"/>
-    </row>
-    <row r="2" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P1" s="4"/>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="18" t="s">
         <v>31</v>
@@ -799,11 +860,15 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="2"/>
+      <c r="M2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P2" s="2"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
@@ -820,10 +885,12 @@
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
-      <c r="N3" s="2"/>
+      <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P3" s="2"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
@@ -851,10 +918,12 @@
       </c>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
-      <c r="N4" s="2"/>
+      <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P4" s="2"/>
+      <c r="Q4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>22</v>
       </c>
@@ -878,10 +947,12 @@
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="2"/>
+      <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P5" s="2"/>
+      <c r="Q5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>34</v>
       </c>
@@ -906,13 +977,15 @@
       <c r="L6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P6" s="2"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
@@ -932,10 +1005,12 @@
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
-      <c r="N7" s="2"/>
+      <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P7" s="2"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -957,13 +1032,12 @@
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
-      <c r="N8" s="2"/>
+      <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="P8" s="2"/>
+      <c r="Q8" s="1"/>
+    </row>
+    <row r="9" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1" t="s">
@@ -983,10 +1057,12 @@
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
-      <c r="N9" s="2"/>
+      <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P9" s="2"/>
+      <c r="Q9" s="1"/>
+    </row>
+    <row r="10" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>51</v>
       </c>
@@ -1001,67 +1077,69 @@
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J10" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="2"/>
+      <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P10" s="2"/>
+      <c r="Q10" s="1"/>
+    </row>
+    <row r="11" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>53</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
-      <c r="N11" s="2"/>
+      <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P11" s="2"/>
+      <c r="Q11" s="1"/>
+    </row>
+    <row r="12" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>28</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>53</v>
@@ -1070,12 +1148,14 @@
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
-      <c r="N12" s="2"/>
+      <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P12" s="2"/>
+      <c r="Q12" s="1"/>
+    </row>
+    <row r="13" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1086,56 +1166,94 @@
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="K13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="2"/>
+      <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
+      <c r="P13" s="2"/>
+      <c r="Q13" s="1"/>
+    </row>
+    <row r="14" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-      <c r="N14" s="2"/>
+      <c r="L14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="1"/>
+    </row>
+    <row r="15" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>78</v>
+      </c>
       <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
+      <c r="F15" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
+      <c r="H15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>75</v>
+      </c>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
-      <c r="N15" s="3"/>
-    </row>
-    <row r="16" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="N15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O15" s="1"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1149,12 +1267,14 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
-      <c r="N16" s="2" t="s">
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="Q16" s="1"/>
+    </row>
+    <row r="17" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1168,14 +1288,16 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="2" t="s">
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="Q17" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1189,14 +1311,16 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="2" t="s">
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="Q18" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1210,14 +1334,16 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="2" t="s">
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O19" s="1" t="s">
+      <c r="Q19" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1231,14 +1357,16 @@
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
-      <c r="N20" s="2" t="s">
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="Q20" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1252,14 +1380,16 @@
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="2" t="s">
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="Q21" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1273,14 +1403,16 @@
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="2" t="s">
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O22" s="1" t="s">
+      <c r="Q22" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1294,73 +1426,85 @@
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
-      <c r="N23" s="2" t="s">
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O23" s="1" t="s">
+      <c r="Q23" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="N24" s="2" t="s">
+    <row r="24" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P24" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="Q24" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="N25" s="2" t="s">
+    <row r="25" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="O25" s="1" t="s">
+      <c r="Q25" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="N26" s="3" t="s">
+    <row r="26" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P26" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="O26" s="1" t="s">
+      <c r="Q26" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="N27" s="20" t="s">
+    <row r="27" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P27" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="O27" s="1" t="s">
+      <c r="Q27" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:15" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="N28" s="20" t="s">
+    <row r="28" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P28" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="O28" s="1" t="s">
+      <c r="Q28" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="N29" s="3"/>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="N30" s="3"/>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="N31" s="3"/>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="N32" s="3"/>
-    </row>
-    <row r="33" spans="14:14" x14ac:dyDescent="0.2">
-      <c r="N33" s="3"/>
-    </row>
-    <row r="34" spans="14:14" x14ac:dyDescent="0.2">
-      <c r="N34" s="3"/>
-    </row>
-    <row r="35" spans="14:14" x14ac:dyDescent="0.2">
-      <c r="N35" s="3"/>
+    <row r="29" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="P30" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P31" s="3"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="P32" s="3"/>
+    </row>
+    <row r="33" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P33" s="3"/>
+    </row>
+    <row r="34" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P34" s="3"/>
+    </row>
+    <row r="35" spans="16:16" x14ac:dyDescent="0.2">
+      <c r="P35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>